<commit_message>
Doxygen adapted & Novec comparison added
</commit_message>
<xml_diff>
--- a/documents/Halon1301_container_discharge.xlsx
+++ b/documents/Halon1301_container_discharge.xlsx
@@ -104,10 +104,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1296,11 +1296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="308134704"/>
-        <c:axId val="308134312"/>
+        <c:axId val="567094008"/>
+        <c:axId val="567094400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="308134704"/>
+        <c:axId val="567094008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,12 +1413,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308134312"/>
+        <c:crossAx val="567094400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="308134312"/>
+        <c:axId val="567094400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1532,7 +1532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308134704"/>
+        <c:crossAx val="567094008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -3845,11 +3845,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="318946336"/>
-        <c:axId val="318945552"/>
+        <c:axId val="567095184"/>
+        <c:axId val="567095576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="318946336"/>
+        <c:axId val="567095184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3962,12 +3962,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318945552"/>
+        <c:crossAx val="567095576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="318945552"/>
+        <c:axId val="567095576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -4081,7 +4081,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="318946336"/>
+        <c:crossAx val="567095184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -5348,6 +5348,67 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>349251</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>243417</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12319001" y="11398250"/>
+          <a:ext cx="2243666" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Agreement with NFPA data.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9331,8 +9392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" topLeftCell="E40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O63" sqref="O63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9360,66 +9421,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="N1" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="2"/>
-      <c r="N2" s="2" t="s">
+      <c r="J2" s="3"/>
+      <c r="N2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2" t="s">
+      <c r="O2" s="3"/>
+      <c r="P2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2" t="s">
+      <c r="S2" s="3"/>
+      <c r="T2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U2" s="2"/>
+      <c r="U2" s="3"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">

</xml_diff>

<commit_message>
Heat capacity ratio data added
</commit_message>
<xml_diff>
--- a/documents/Halon1301_container_discharge.xlsx
+++ b/documents/Halon1301_container_discharge.xlsx
@@ -1296,11 +1296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="567094008"/>
-        <c:axId val="567094400"/>
+        <c:axId val="322001040"/>
+        <c:axId val="322001432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="567094008"/>
+        <c:axId val="322001040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,12 +1413,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567094400"/>
+        <c:crossAx val="322001432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="567094400"/>
+        <c:axId val="322001432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1532,7 +1532,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567094008"/>
+        <c:crossAx val="322001040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -1657,13 +1657,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Comparison</a:t>
+              <a:rPr lang="en-US" sz="2000" b="1"/>
+              <a:t>Halon Discharge Container States Comparison</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.15081160241851504"/>
+          <c:y val="2.3024508799687551E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1703,7 +1710,7 @@
           <c:idx val="4"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Density80</c:v>
+            <c:v>Density=80 Own Code</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -1955,7 +1962,7 @@
           <c:idx val="0"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Density70</c:v>
+            <c:v>Density=70 Own Code</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2189,7 +2196,7 @@
           <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Density60</c:v>
+            <c:v>Density=60 Own Code</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2411,7 +2418,7 @@
           <c:idx val="2"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Density50</c:v>
+            <c:v>Density=50 Own Code</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2609,7 +2616,7 @@
           <c:idx val="3"/>
           <c:order val="4"/>
           <c:tx>
-            <c:v>Density40</c:v>
+            <c:v>Density=40 Own Code</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -2783,7 +2790,7 @@
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
-            <c:v>Density70Data</c:v>
+            <c:v>Density=70 NFPA Data</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3037,7 +3044,7 @@
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
-            <c:v>Density60Data</c:v>
+            <c:v>Density=60 NFPA Data</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3305,7 +3312,7 @@
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
-            <c:v>Density50Data</c:v>
+            <c:v>Density=50 NFPA Data</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3573,7 +3580,7 @@
           <c:idx val="8"/>
           <c:order val="8"/>
           <c:tx>
-            <c:v>Density40Data</c:v>
+            <c:v>Density=40 NFPA Data</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
@@ -3845,11 +3852,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="567095184"/>
-        <c:axId val="567095576"/>
+        <c:axId val="322002216"/>
+        <c:axId val="322002608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="567095184"/>
+        <c:axId val="322002216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3889,7 +3896,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Percent Outage</a:t>
                 </a:r>
               </a:p>
@@ -3947,7 +3954,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3962,12 +3969,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567095576"/>
+        <c:crossAx val="322002608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="567095576"/>
+        <c:axId val="322002608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -4008,13 +4015,20 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="1600"/>
                   <a:t>Container Pressure (psig)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.282051282051282E-2"/>
+              <c:y val="0.21354038589587607"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4066,7 +4080,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4081,7 +4095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="567095184"/>
+        <c:crossAx val="322002216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
@@ -4096,13 +4110,36 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.7916453214432528E-2"/>
-          <c:y val="0.3101310070133389"/>
-          <c:w val="0.13415101958409045"/>
+          <c:x val="9.1054588945795767E-2"/>
+          <c:y val="0.31433399249551858"/>
+          <c:w val="0.20276919180108985"/>
           <c:h val="0.51724506890116662"/>
         </c:manualLayout>
       </c:layout>
@@ -4119,7 +4156,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -4169,6 +4206,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -5318,16 +5356,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>387308</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>747142</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>160564</xdr:rowOff>
+      <xdr:rowOff>158751</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>882608</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>79601</xdr:rowOff>
+      <xdr:colOff>1471083</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5350,16 +5388,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>349251</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>952503</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>74084</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>243417</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381002</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>35984</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -5368,7 +5406,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12319001" y="11398250"/>
+          <a:off x="11842753" y="12139084"/>
           <a:ext cx="2243666" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5410,6 +5448,126 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.61917</cdr:x>
+      <cdr:y>0.76611</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.793</cdr:x>
+      <cdr:y>0.83294</cdr:y>
+    </cdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <cdr:sp macro="" textlink="">
+          <cdr:nvSpPr>
+            <cdr:cNvPr id="2" name="TextBox 1"/>
+            <cdr:cNvSpPr txBox="1"/>
+          </cdr:nvSpPr>
+          <cdr:spPr>
+            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:off x="5729859" y="3397252"/>
+              <a:ext cx="1608666" cy="296333"/>
+            </a:xfrm>
+            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </cdr:spPr>
+          <cdr:txBody>
+            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:r>
+                <a:rPr lang="en-US" sz="1200"/>
+                <a:t>Density unit </a:t>
+              </a:r>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>𝑙𝑏𝑠</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>/</m:t>
+                  </m:r>
+                  <m:sSup>
+                    <m:sSupPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSupPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑓𝑡</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sup>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>3</m:t>
+                      </m:r>
+                    </m:sup>
+                  </m:sSup>
+                </m:oMath>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1200"/>
+            </a:p>
+          </cdr:txBody>
+        </cdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <cdr:sp macro="" textlink="">
+          <cdr:nvSpPr>
+            <cdr:cNvPr id="2" name="TextBox 1"/>
+            <cdr:cNvSpPr txBox="1"/>
+          </cdr:nvSpPr>
+          <cdr:spPr>
+            <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:off x="5729859" y="3397252"/>
+              <a:ext cx="1608666" cy="296333"/>
+            </a:xfrm>
+            <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </cdr:spPr>
+          <cdr:txBody>
+            <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+            <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+            <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:r>
+                <a:rPr lang="en-US" sz="1200"/>
+                <a:t>Density unit </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑙𝑏𝑠/〖𝑓𝑡〗^3</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1200"/>
+            </a:p>
+          </cdr:txBody>
+        </cdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5677,7 +5835,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B34"/>
     </sheetView>
   </sheetViews>
@@ -9392,8 +9550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O63" sqref="O63"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>